<commit_message>
Fix minor bugs with file structure
</commit_message>
<xml_diff>
--- a/Origin_parameters_plot.xlsx
+++ b/Origin_parameters_plot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\a PSI\Data\Data analysis\XPEEM_toolkit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5724AA95-9985-4A49-9996-F7E9294087E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF94E19-7AE0-4BE2-A60D-F840C698C218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4BE89B8D-14F3-48DA-B536-D8C3A73E6BE2}"/>
   </bookViews>
@@ -531,6 +531,9 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -559,6 +562,39 @@
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -650,42 +686,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -734,7 +734,7 @@
     <tableColumn id="3" xr3:uid="{3A12CF31-CDCB-4C3F-8981-47758C1FE96E}" name="typePlot"/>
     <tableColumn id="1" xr3:uid="{412C3A9C-C485-4181-AF50-F1543CE684DD}" name="graphTitles"/>
     <tableColumn id="23" xr3:uid="{8856B606-4F5A-4250-9465-68E4265AB536}" name="colUnit"/>
-    <tableColumn id="25" xr3:uid="{02A23255-F19C-4EC1-9539-EC9E4039D53F}" name="templategraph" dataDxfId="16">
+    <tableColumn id="25" xr3:uid="{02A23255-F19C-4EC1-9539-EC9E4039D53F}" name="templategraph" dataDxfId="7">
       <calculatedColumnFormula>CONCATENATE(Table1[[#This Row],[Exp]],"/",Table1[[#This Row],[templatefile]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -755,7 +755,7 @@
     <tableColumn id="8" xr3:uid="{EA827503-2BB8-4325-9A30-099B9411A38D}" name="templatefile"/>
     <tableColumn id="10" xr3:uid="{87575AD2-5830-4469-BBBD-83A3D01FB1F8}" name="pixel_size"/>
     <tableColumn id="5" xr3:uid="{CA2FD2C4-AE5B-4101-B7DF-73520F187D89}" name="unit"/>
-    <tableColumn id="1" xr3:uid="{DE1F3DA3-C241-40D6-B061-772710D29CCE}" name="templategraph" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{DE1F3DA3-C241-40D6-B061-772710D29CCE}" name="templategraph" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.CONCAT(Table13[[#This Row],[Exp]],"/",Table13[[#This Row],[templatefile]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1064,7 +1064,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G25" sqref="G25"/>
+      <selection pane="topRight" activeCell="J20" sqref="J17:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,7 +1077,7 @@
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.140625" customWidth="1"/>
-    <col min="10" max="10" width="28" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -2881,35 +2881,35 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A30:XFD1048576 A1:S1 A2:XFD26 U1:XFD1 T27:T28 U27:XFD29 A27:S29">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
       <formula>"None"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>"None"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T29">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>"None"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3206,24 +3206,24 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A1:G1 A3:G3 H1:XFD3 E2:G2 A4:XFD1048576">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"None"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F2">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"None"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>